<commit_message>
readme update + formatting + bug + other corrections
</commit_message>
<xml_diff>
--- a/tests/Test_Specification.xlsx
+++ b/tests/Test_Specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Essa\Documents\GitHub\ETL_Stock_project\ETL_stock_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3896EAEB-EAEC-4B21-9045-97940E547304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006A3792-167C-4A15-9C0B-4AB77EEF8BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B063D267-4ADC-4DCE-AB62-3AD5DB7A94EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B063D267-4ADC-4DCE-AB62-3AD5DB7A94EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -514,18 +514,18 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="18.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.36328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.54296875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="46.1796875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="32.26953125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="32.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -548,7 +548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -571,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="63.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -590,7 +590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -599,7 +599,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
@@ -608,7 +608,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
@@ -617,7 +617,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
@@ -626,7 +626,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="2"/>
@@ -635,7 +635,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
@@ -644,7 +644,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
@@ -653,7 +653,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
@@ -662,7 +662,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
@@ -671,7 +671,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
@@ -680,7 +680,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
@@ -689,7 +689,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
@@ -698,7 +698,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -707,7 +707,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
@@ -716,7 +716,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
@@ -725,7 +725,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
@@ -734,7 +734,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
@@ -743,7 +743,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
@@ -752,7 +752,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -761,7 +761,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
@@ -770,7 +770,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
@@ -779,7 +779,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
@@ -788,7 +788,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
@@ -797,7 +797,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
@@ -806,7 +806,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
@@ -815,7 +815,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2"/>
@@ -824,7 +824,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
@@ -833,7 +833,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
@@ -842,7 +842,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
@@ -851,7 +851,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="2"/>
@@ -860,7 +860,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
@@ -869,7 +869,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="2"/>
@@ -878,7 +878,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="2"/>
@@ -887,7 +887,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2"/>
@@ -896,7 +896,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2"/>
@@ -905,7 +905,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2"/>
@@ -914,7 +914,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="2"/>
@@ -923,7 +923,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="2"/>
@@ -932,7 +932,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="2"/>
@@ -941,7 +941,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="2"/>
@@ -950,7 +950,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="2"/>
@@ -959,7 +959,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2"/>
@@ -968,7 +968,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2"/>
@@ -977,7 +977,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2"/>
@@ -986,7 +986,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
@@ -995,7 +995,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
@@ -1004,7 +1004,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
@@ -1013,7 +1013,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
@@ -1022,7 +1022,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
@@ -1031,7 +1031,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
@@ -1040,7 +1040,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
@@ -1049,7 +1049,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
@@ -1058,7 +1058,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="2"/>
@@ -1067,7 +1067,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="4"/>

</xml_diff>